<commit_message>
Added figure 6 script
</commit_message>
<xml_diff>
--- a/data/single_cell_data.xlsx
+++ b/data/single_cell_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidfandrei/Desktop/PPM1D/publication/Fandrei_et_al_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3F5899-272D-3E4B-92C6-5A971E629009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B5CAE7-52A9-7147-897C-7C94C5E3C784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18100" xr2:uid="{1E9E870A-E523-BF4C-9F88-2291DF3EC000}"/>
   </bookViews>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="657">
   <si>
     <t>id</t>
   </si>
@@ -2092,6 +2092,9 @@
   </si>
   <si>
     <t>M187_chr8_117859807</t>
+  </si>
+  <si>
+    <t>tapestri_id</t>
   </si>
 </sst>
 </file>
@@ -2480,9 +2483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BF59E7-4666-B742-A2A2-96CD398ACCB2}">
-  <dimension ref="A1:AF29"/>
+  <dimension ref="A1:AG29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2514,9 +2519,10 @@
     <col min="30" max="30" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2613,8 +2619,11 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="AG1" s="1" t="s">
+        <v>656</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -2711,8 +2720,11 @@
       <c r="AF2" t="s">
         <v>49</v>
       </c>
+      <c r="AG2" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -2809,8 +2821,11 @@
       <c r="AF3" t="s">
         <v>49</v>
       </c>
+      <c r="AG3" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -2907,8 +2922,11 @@
       <c r="AF4" t="s">
         <v>74</v>
       </c>
+      <c r="AG4" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -3005,8 +3023,11 @@
       <c r="AF5" t="s">
         <v>74</v>
       </c>
+      <c r="AG5" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -3103,8 +3124,11 @@
       <c r="AF6" t="s">
         <v>91</v>
       </c>
+      <c r="AG6" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -3201,8 +3225,11 @@
       <c r="AF7" t="s">
         <v>103</v>
       </c>
+      <c r="AG7" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -3299,8 +3326,11 @@
       <c r="AF8" t="s">
         <v>113</v>
       </c>
+      <c r="AG8" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -3397,8 +3427,11 @@
       <c r="AF9" t="s">
         <v>114</v>
       </c>
+      <c r="AG9" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3495,8 +3528,11 @@
       <c r="AF10" t="s">
         <v>74</v>
       </c>
+      <c r="AG10" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3593,8 +3629,11 @@
       <c r="AF11" t="s">
         <v>49</v>
       </c>
+      <c r="AG11" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -3691,8 +3730,11 @@
       <c r="AF12" t="s">
         <v>113</v>
       </c>
+      <c r="AG12" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -3789,8 +3831,11 @@
       <c r="AF13" t="s">
         <v>114</v>
       </c>
+      <c r="AG13" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>136</v>
       </c>
@@ -3887,8 +3932,11 @@
       <c r="AF14" t="s">
         <v>146</v>
       </c>
+      <c r="AG14" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -3985,8 +4033,11 @@
       <c r="AF15" t="s">
         <v>74</v>
       </c>
+      <c r="AG15" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -4080,8 +4131,11 @@
       <c r="AE16">
         <v>30.6010383386581</v>
       </c>
+      <c r="AG16" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -4178,8 +4232,11 @@
       <c r="AF17" t="s">
         <v>170</v>
       </c>
+      <c r="AG17" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -4276,8 +4333,11 @@
       <c r="AF18" t="s">
         <v>180</v>
       </c>
+      <c r="AG18" t="s">
+        <v>178</v>
+      </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -4374,8 +4434,11 @@
       <c r="AF19" t="s">
         <v>74</v>
       </c>
+      <c r="AG19" t="s">
+        <v>178</v>
+      </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>183</v>
       </c>
@@ -4472,8 +4535,11 @@
       <c r="AF20" t="s">
         <v>194</v>
       </c>
+      <c r="AG20" t="s">
+        <v>192</v>
+      </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>195</v>
       </c>
@@ -4570,8 +4636,11 @@
       <c r="AF21" t="s">
         <v>74</v>
       </c>
+      <c r="AG21" t="s">
+        <v>192</v>
+      </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>199</v>
       </c>
@@ -4668,8 +4737,11 @@
       <c r="AF22" t="s">
         <v>208</v>
       </c>
+      <c r="AG22" t="s">
+        <v>206</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>209</v>
       </c>
@@ -4763,8 +4835,11 @@
       <c r="AE23">
         <v>21.8088151116199</v>
       </c>
+      <c r="AG23" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>220</v>
       </c>
@@ -4861,8 +4936,11 @@
       <c r="AF24" t="s">
         <v>74</v>
       </c>
+      <c r="AG24" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>226</v>
       </c>
@@ -4959,8 +5037,11 @@
       <c r="AF25" t="s">
         <v>194</v>
       </c>
+      <c r="AG25" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -5057,8 +5138,11 @@
       <c r="AF26" t="s">
         <v>49</v>
       </c>
+      <c r="AG26" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>238</v>
       </c>
@@ -5155,8 +5239,11 @@
       <c r="AF27" t="s">
         <v>194</v>
       </c>
+      <c r="AG27" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>246</v>
       </c>
@@ -5247,8 +5334,11 @@
       <c r="AF28" t="s">
         <v>74</v>
       </c>
+      <c r="AG28" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>209</v>
       </c>
@@ -5341,6 +5431,9 @@
       </c>
       <c r="AE29">
         <v>15.068302202397501</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>